<commit_message>
modified the family expenses
</commit_message>
<xml_diff>
--- a/Family_Expenses.xlsx
+++ b/Family_Expenses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VINAYTECH_CLASSROOM_TEACHING_INFO\POWER BI\VINAYTECH_POWER BI_FILES_DATABASES_BACKUP_RESTORE_DOC\GENERAL FILES FOR PRACTICE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\mahesh_training_data-test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8F4550-D738-4814-BAFA-649CDC0F33A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCCA356-DD70-4235-A467-91EF62F36E69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16605" windowHeight="8835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -158,7 +158,7 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -513,19 +513,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:E56"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -542,7 +542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -559,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44060</v>
       </c>
@@ -576,7 +576,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44059</v>
       </c>
@@ -593,7 +593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44060</v>
       </c>
@@ -610,7 +610,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44061</v>
       </c>
@@ -627,7 +627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44062</v>
       </c>
@@ -644,7 +644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44063</v>
       </c>
@@ -661,7 +661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44064</v>
       </c>
@@ -678,7 +678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44065</v>
       </c>
@@ -695,7 +695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44066</v>
       </c>
@@ -712,7 +712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44067</v>
       </c>
@@ -729,7 +729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44068</v>
       </c>
@@ -746,7 +746,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44014</v>
       </c>
@@ -763,7 +763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44015</v>
       </c>
@@ -780,7 +780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44016</v>
       </c>
@@ -797,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44017</v>
       </c>
@@ -814,7 +814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44018</v>
       </c>
@@ -831,7 +831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44019</v>
       </c>
@@ -848,7 +848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44020</v>
       </c>
@@ -865,7 +865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44021</v>
       </c>
@@ -882,7 +882,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44022</v>
       </c>
@@ -899,7 +899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44060</v>
       </c>
@@ -916,7 +916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44059</v>
       </c>
@@ -933,7 +933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44060</v>
       </c>
@@ -950,7 +950,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44061</v>
       </c>
@@ -967,7 +967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44062</v>
       </c>
@@ -984,7 +984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44063</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44064</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44065</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44066</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44067</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44068</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44014</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44015</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44016</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44017</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44018</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44019</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44020</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44021</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44022</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43694</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43693</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43695</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43688</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43696</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43697</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43698</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43699</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43700</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43701</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43702</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43648</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43649</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43650</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43651</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43652</v>
       </c>
@@ -1504,8 +1504,11 @@
       <c r="D58" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43653</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43654</v>
       </c>
@@ -1532,8 +1535,11 @@
       <c r="D60" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43655</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43656</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43694</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43693</v>
       </c>
@@ -1595,7 +1601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43694</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43695</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43696</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43697</v>
       </c>
@@ -1650,8 +1656,11 @@
       <c r="D68" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43698</v>
       </c>
@@ -1665,7 +1674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43699</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43700</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43701</v>
       </c>
@@ -1707,7 +1716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43702</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43648</v>
       </c>
@@ -1735,7 +1744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43649</v>
       </c>
@@ -1749,7 +1758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43650</v>
       </c>
@@ -1763,7 +1772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43651</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43652</v>
       </c>
@@ -1791,7 +1800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43653</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43654</v>
       </c>
@@ -1819,7 +1828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43655</v>
       </c>
@@ -1833,7 +1842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43656</v>
       </c>
@@ -1864,12 +1873,12 @@
       <selection sqref="A1:F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43694</v>
       </c>
@@ -1886,7 +1895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43693</v>
       </c>
@@ -1903,7 +1912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43694</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43695</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43696</v>
       </c>
@@ -1945,7 +1954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43697</v>
       </c>
@@ -1959,7 +1968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43698</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43699</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43700</v>
       </c>
@@ -2001,7 +2010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43701</v>
       </c>
@@ -2015,7 +2024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43702</v>
       </c>
@@ -2029,7 +2038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43648</v>
       </c>
@@ -2043,7 +2052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43649</v>
       </c>
@@ -2057,7 +2066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43650</v>
       </c>
@@ -2071,7 +2080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43651</v>
       </c>
@@ -2085,7 +2094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43652</v>
       </c>
@@ -2099,7 +2108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43653</v>
       </c>
@@ -2113,7 +2122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43654</v>
       </c>
@@ -2127,7 +2136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43655</v>
       </c>
@@ -2141,7 +2150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43656</v>
       </c>
@@ -2155,7 +2164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43694</v>
       </c>
@@ -2172,7 +2181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43693</v>
       </c>
@@ -2189,7 +2198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43694</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43695</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43696</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43697</v>
       </c>
@@ -2245,7 +2254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43698</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43699</v>
       </c>
@@ -2273,7 +2282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43700</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43701</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43702</v>
       </c>
@@ -2315,7 +2324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43648</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43649</v>
       </c>
@@ -2343,7 +2352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43650</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43651</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43652</v>
       </c>
@@ -2385,7 +2394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43653</v>
       </c>
@@ -2399,7 +2408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43654</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43655</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43656</v>
       </c>
@@ -2452,7 +2461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>